<commit_message>
Login Module (Front End)
</commit_message>
<xml_diff>
--- a/Test Cases for login Module.xlsx
+++ b/Test Cases for login Module.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Angular Projects\Online-Examinination-System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373F1745-C2AA-49FB-B537-301FC05BA87D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F3F428-760C-49AF-96DB-90D178EBE716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Test Cases For Login Module</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>3. Add Forgot Password Option</t>
+  </si>
+  <si>
+    <t>1. Correct Username</t>
+  </si>
+  <si>
+    <t>2. New Password and Confirmed New Password should be equal.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Test Cases for Forgot Password</t>
   </si>
 </sst>
 </file>
@@ -370,16 +379,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="58.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
@@ -416,6 +425,21 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>